<commit_message>
All HashCode and equals
</commit_message>
<xml_diff>
--- a/ES. checklist_es.xlsx
+++ b/ES. checklist_es.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1Escritorio\Informatica\Uni\Cuarto Curso\Primer Cuatrimestre\Repositorios de Informacion\Laboratorio\ri-jpa-2020-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B63180A-102F-4385-9514-6C2D143F36B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6555169-159F-4FEF-928D-441C24AD785F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1227,7 +1227,7 @@
   <dimension ref="B2:H80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1337,9 @@
       <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="11">
@@ -1903,7 +1905,7 @@
       </c>
       <c r="D6">
         <f>SUMPRODUCT('check list'!B9:B14,'check list'!D9:D14)</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.2">

</xml_diff>